<commit_message>
update py script 20211024
</commit_message>
<xml_diff>
--- a/Network_List_v1.0.xlsx
+++ b/Network_List_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\James\Desktop\Coding\Python\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2568534A-7D27-4D89-B17E-1E5C580796A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B6B7F2-536C-4E18-91CA-73DB5A178E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,17 +510,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A1:A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>